<commit_message>
made some testing with code. Just commiting.
</commit_message>
<xml_diff>
--- a/utils/documents_data.xlsx
+++ b/utils/documents_data.xlsx
@@ -3,13 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28521"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{188F728D-FF33-42D8-AB9A-B9199AEF933F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B74F6E89-9913-4978-A412-62B1A39A4B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
   <si>
     <t>document_type</t>
   </si>
@@ -55,42 +57,42 @@
     <t>name_matching_text</t>
   </si>
   <si>
+    <t>Commercial Invoice</t>
+  </si>
+  <si>
+    <t>email attachment</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>processing</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Bill of</t>
+  </si>
+  <si>
+    <t>startswith</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Arrival Notice</t>
+  </si>
+  <si>
     <t>Airway Bill</t>
   </si>
   <si>
-    <t>email attachment</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
-    <t>processing</t>
-  </si>
-  <si>
-    <t>english</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Bill of</t>
-  </si>
-  <si>
-    <t>startswith</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>Commercial Invoice</t>
-  </si>
-  <si>
-    <t>auto</t>
-  </si>
-  <si>
-    <t>Arrival Notice</t>
-  </si>
-  <si>
     <t>Bank draft</t>
   </si>
   <si>
@@ -98,6 +100,33 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>key_field_name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>assembly</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>country code</t>
+  </si>
+  <si>
+    <t>consignee city</t>
+  </si>
+  <si>
+    <t>selector</t>
   </si>
 </sst>
 </file>
@@ -467,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -557,7 +586,156 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G6"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BC9590-9E61-4ED1-9189-3F4DB0FEBFAD}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -587,13 +765,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -605,90 +783,63 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A927DA3E-FC2F-4247-8123-4D092A9DF600}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>